<commit_message>
SP MEDICAL GROUP ATUALIZAÇÃO
</commit_message>
<xml_diff>
--- a/sp med. group/modelagens/modelagem-sp-med-group-fisico.xlsx
+++ b/sp med. group/modelagens/modelagem-sp-med-group-fisico.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23906"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23911"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{715AB5BE-9E47-4914-805C-5C158FBFF016}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D1125B0-8EEC-45F6-936C-0A7246D18DBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="114">
   <si>
     <t>tipoUsuario</t>
   </si>
@@ -67,15 +67,9 @@
     <t>Administrador</t>
   </si>
   <si>
-    <t>22033388-9</t>
-  </si>
-  <si>
     <t>Rua Tupanaci 897, Vila Gumercindo, São Paulo, 04131-020</t>
   </si>
   <si>
-    <t>11 2738-5781</t>
-  </si>
-  <si>
     <t>ricardo.lemos@spmedicalgroup.com.br</t>
   </si>
   <si>
@@ -85,15 +79,9 @@
     <t>Paciente</t>
   </si>
   <si>
-    <t>43736451-3</t>
-  </si>
-  <si>
     <t>Rua Lourenço Leite Penteado 303, Parque São Rafael, São Paulo, 08311-170</t>
   </si>
   <si>
-    <t>11 99295-8066</t>
-  </si>
-  <si>
     <t>roberto.possarle@spmedicalgroup.com.br</t>
   </si>
   <si>
@@ -103,114 +91,69 @@
     <t>Médico</t>
   </si>
   <si>
-    <t>16905801-3</t>
-  </si>
-  <si>
     <t>Avenida Presidente Wilson 763, Mooca , São Paulo, 03107-001</t>
   </si>
   <si>
-    <t>11 3929-4920</t>
-  </si>
-  <si>
     <t>helena.souza@spmedicalgroup.com.br</t>
   </si>
   <si>
     <t>helena456</t>
   </si>
   <si>
-    <t>43522543-5</t>
-  </si>
-  <si>
     <t>Rua Estado de Israel 240, São Paulo, Estado de São Paulo, 04022-000</t>
   </si>
   <si>
-    <t>11 3456-7654</t>
-  </si>
-  <si>
     <t>ligia@gmail.com</t>
   </si>
   <si>
     <t>ligia123</t>
   </si>
   <si>
-    <t>32654345-7</t>
-  </si>
-  <si>
     <t>Av. Paulista, 1578 - Bela Vista, São Paulo - SP, 01310-200</t>
   </si>
   <si>
-    <t>11 98765-6543</t>
-  </si>
-  <si>
     <t>alexandre@gmail.com</t>
   </si>
   <si>
     <t>alexandre987</t>
   </si>
   <si>
-    <t>54636525-3</t>
-  </si>
-  <si>
     <t>Av. Ibirapuera - Indianópolis, 2927,  São Paulo - SP, 04029-200</t>
   </si>
   <si>
-    <t>11 97208-4453</t>
-  </si>
-  <si>
     <t>fernando@gmail.com</t>
   </si>
   <si>
     <t>fernando123</t>
   </si>
   <si>
-    <t>54366362-5</t>
-  </si>
-  <si>
     <t>R. Vitória, 120 - Vila Sao Jorge, Barueri - SP, 06402-030</t>
   </si>
   <si>
-    <t>11 3456-6543</t>
-  </si>
-  <si>
     <t>henrique@gmail.com</t>
   </si>
   <si>
     <t>henrique987</t>
   </si>
   <si>
-    <t>532544444-1</t>
-  </si>
-  <si>
     <t>R. Ver. Geraldo de Camargo, 66 - Santa Luzia, Ribeirão Pires - SP, 09405-380</t>
   </si>
   <si>
-    <t>11 7656-6377</t>
-  </si>
-  <si>
     <t>joao@hotmail.com</t>
   </si>
   <si>
     <t>joao123</t>
   </si>
   <si>
-    <t>54566266-7</t>
-  </si>
-  <si>
     <t>Alameda dos Arapanés, 945 - Indianópolis, São Paulo - SP, 04524-001</t>
   </si>
   <si>
-    <t>11 95436-8769</t>
-  </si>
-  <si>
     <t>bruno@gmail.com</t>
   </si>
   <si>
     <t>bruno987</t>
   </si>
   <si>
-    <t>54566266-8</t>
-  </si>
-  <si>
     <t>R Sao Antonio, 232 - Vila Universal, Barueri - SP, 06407-140</t>
   </si>
   <si>
@@ -220,30 +163,18 @@
     <t>mariana123</t>
   </si>
   <si>
-    <t>43453872-3</t>
-  </si>
-  <si>
     <t>Rua Genésio dos Santos 465, Vila Granada, São Paulo, 03654-110</t>
   </si>
   <si>
-    <t>11 99791-4517</t>
-  </si>
-  <si>
     <t>isabellyreginabaptista__@spmedicalgroup.com.br</t>
   </si>
   <si>
     <t>mBCohJ4fle</t>
   </si>
   <si>
-    <t>32288728-8</t>
-  </si>
-  <si>
     <t>Avenida Presidente Wilson 1230, Mooca, São Paulo, 03107-901</t>
   </si>
   <si>
-    <t>11 99300-9597</t>
-  </si>
-  <si>
     <t>tomasrenatoenzobarros_@spmedicalgroup.com.br</t>
   </si>
   <si>
@@ -286,7 +217,7 @@
     <t>Ricardo Lemos</t>
   </si>
   <si>
-    <t>54356-SP</t>
+    <t>54356SP</t>
   </si>
   <si>
     <t>Av. Barão Limeira, 532, São Paulo, SP</t>
@@ -295,9 +226,6 @@
     <t>07:00 às 22:00</t>
   </si>
   <si>
-    <t>86.400.902/0001-30</t>
-  </si>
-  <si>
     <t xml:space="preserve">Clinica Possarle </t>
   </si>
   <si>
@@ -307,13 +235,13 @@
     <t>Roberto Possarle</t>
   </si>
   <si>
-    <t>53452-SP</t>
+    <t>53452SP</t>
   </si>
   <si>
     <t>Helena Strada</t>
   </si>
   <si>
-    <t>65463-SP</t>
+    <t>65463SP</t>
   </si>
   <si>
     <t>especialidade</t>
@@ -404,9 +332,6 @@
   </si>
   <si>
     <t>idConsulta</t>
-  </si>
-  <si>
-    <t>idProntuario</t>
   </si>
   <si>
     <t>dataAgendamento</t>
@@ -613,21 +538,12 @@
     <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -637,9 +553,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -648,9 +561,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -667,8 +577,23 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -987,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1010,23 +935,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -1096,26 +1021,26 @@
       <c r="F3" s="6">
         <v>3</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>13</v>
+      <c r="G3" s="6">
+        <v>220333889</v>
       </c>
       <c r="H3" s="6">
         <v>37182407850</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="9">
         <v>33369</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="6">
+        <v>1127385781</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1131,7 +1056,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2"/>
       <c r="E4" s="6">
@@ -1140,26 +1065,26 @@
       <c r="F4" s="6">
         <v>3</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>19</v>
+      <c r="G4" s="6">
+        <v>437364513</v>
       </c>
       <c r="H4" s="6">
         <v>38093066810</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J4" s="9">
         <v>28683</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>21</v>
+      <c r="K4" s="6">
+        <v>11992958066</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -1175,7 +1100,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2"/>
       <c r="E5" s="6">
@@ -1184,26 +1109,26 @@
       <c r="F5" s="6">
         <v>3</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>25</v>
+      <c r="G5" s="6">
+        <v>169058013</v>
       </c>
       <c r="H5" s="6">
         <v>89610795811</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J5" s="9">
         <v>34495</v>
       </c>
-      <c r="K5" s="6" t="s">
-        <v>27</v>
+      <c r="K5" s="6">
+        <v>1139294920</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1224,26 +1149,26 @@
       <c r="F6" s="6">
         <v>2</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>30</v>
+      <c r="G6" s="6">
+        <v>435225435</v>
       </c>
       <c r="H6" s="6">
         <v>94839859000</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="J6" s="9">
         <v>30602</v>
       </c>
-      <c r="K6" s="6" t="s">
-        <v>32</v>
+      <c r="K6" s="6">
+        <v>1134567654</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1264,26 +1189,26 @@
       <c r="F7" s="6">
         <v>2</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>35</v>
+      <c r="G7" s="6">
+        <v>326543457</v>
       </c>
       <c r="H7" s="6">
         <v>73556944057</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J7" s="9">
         <v>37095</v>
       </c>
-      <c r="K7" s="6" t="s">
-        <v>37</v>
+      <c r="K7" s="6">
+        <v>11987656543</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1304,26 +1229,26 @@
       <c r="F8" s="6">
         <v>2</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>40</v>
+      <c r="G8" s="6">
+        <v>546365253</v>
       </c>
       <c r="H8" s="6">
         <v>16839338002</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="J8" s="9">
         <v>28773</v>
       </c>
-      <c r="K8" s="6" t="s">
-        <v>42</v>
+      <c r="K8" s="6">
+        <v>11972084453</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -1344,26 +1269,26 @@
       <c r="F9" s="6">
         <v>2</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>45</v>
+      <c r="G9" s="6">
+        <v>543663625</v>
       </c>
       <c r="H9" s="6">
         <v>14332654765</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="J9" s="9">
         <v>31333</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>47</v>
+      <c r="K9" s="6">
+        <v>1134566543</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1384,26 +1309,26 @@
       <c r="F10" s="6">
         <v>2</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>50</v>
+      <c r="G10" s="6">
+        <v>5325444441</v>
       </c>
       <c r="H10" s="6">
         <v>91305348010</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="J10" s="9">
         <v>27633</v>
       </c>
-      <c r="K10" s="6" t="s">
-        <v>52</v>
+      <c r="K10" s="6">
+        <v>1176566377</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1424,26 +1349,26 @@
       <c r="F11" s="6">
         <v>2</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>55</v>
+      <c r="G11" s="6">
+        <v>545662667</v>
       </c>
       <c r="H11" s="6">
         <v>79799299004</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="J11" s="9">
         <v>26379</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>57</v>
+      <c r="K11" s="6">
+        <v>11954368769</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1464,24 +1389,24 @@
       <c r="F12" s="6">
         <v>2</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>60</v>
+      <c r="G12" s="6">
+        <v>545662668</v>
       </c>
       <c r="H12" s="6">
         <v>13771913039</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="J12" s="9">
         <v>43164</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="7" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1502,26 +1427,26 @@
       <c r="F13" s="6">
         <v>1</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>64</v>
+      <c r="G13" s="6">
+        <v>434538723</v>
       </c>
       <c r="H13" s="6">
         <v>5129450809</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="J13" s="9">
         <v>34500</v>
       </c>
-      <c r="K13" s="6" t="s">
-        <v>66</v>
+      <c r="K13" s="6">
+        <v>11997914517</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1542,26 +1467,26 @@
       <c r="F14" s="6">
         <v>1</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>69</v>
+      <c r="G14" s="6">
+        <v>322887288</v>
       </c>
       <c r="H14" s="6">
         <v>83193775878</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="J14" s="9">
         <v>35156</v>
       </c>
-      <c r="K14" s="6" t="s">
-        <v>71</v>
+      <c r="K14" s="6">
+        <v>11993009597</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -1642,23 +1567,23 @@
       <c r="U17" s="2"/>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="A18" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
+      <c r="H18" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -1669,42 +1594,42 @@
       <c r="U18" s="2"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="12" t="s">
+      <c r="A19" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>80</v>
+      <c r="D19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="I19" s="16" t="s">
+      <c r="H19" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J19" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="M19" s="16" t="s">
-        <v>84</v>
+      <c r="J19" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -1716,42 +1641,42 @@
       <c r="U19" s="2"/>
     </row>
     <row r="20" spans="1:21">
-      <c r="A20" s="13">
+      <c r="A20" s="11">
         <v>1</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="11">
         <v>1</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="11">
         <v>3</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="11">
         <v>2</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>86</v>
+      <c r="E20" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="17">
+      <c r="H20" s="14">
         <v>1</v>
       </c>
-      <c r="I20" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="L20" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="M20" s="17" t="s">
-        <v>91</v>
+      <c r="I20" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="K20" s="14">
+        <v>86400902000130</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -1763,23 +1688,23 @@
       <c r="U20" s="2"/>
     </row>
     <row r="21" spans="1:21">
-      <c r="A21" s="13">
+      <c r="A21" s="11">
         <v>2</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="11">
         <v>1</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="11">
         <v>3</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="11">
         <v>17</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>93</v>
+      <c r="E21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1798,23 +1723,23 @@
       <c r="U21" s="2"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="13">
+      <c r="A22" s="11">
         <v>3</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="11">
         <v>1</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="11">
         <v>3</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="11">
         <v>16</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>95</v>
+      <c r="E22" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1833,12 +1758,12 @@
       <c r="U22" s="2"/>
     </row>
     <row r="23" spans="1:21">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1856,23 +1781,23 @@
       <c r="U23" s="2"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
+      <c r="A24" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
@@ -1882,34 +1807,34 @@
       <c r="U24" s="2"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="21" t="s">
+      <c r="A25" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="16" t="s">
+      <c r="C25" s="12"/>
+      <c r="D25" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="H25" s="15"/>
-      <c r="I25" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="J25" s="29" t="s">
+      <c r="F25" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="J25" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="K25" s="29" t="s">
-        <v>79</v>
+      <c r="K25" s="24" t="s">
+        <v>56</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
@@ -1920,34 +1845,34 @@
       <c r="U25" s="2"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="20">
+      <c r="A26" s="16">
         <v>1</v>
       </c>
-      <c r="B26" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="17">
+      <c r="B26" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="14">
         <v>1</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="14">
         <v>4</v>
       </c>
-      <c r="F26" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H26" s="15"/>
-      <c r="I26" s="28">
+      <c r="F26" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H26" s="12"/>
+      <c r="I26" s="23">
         <v>1</v>
       </c>
-      <c r="J26" s="28">
+      <c r="J26" s="23">
         <v>11</v>
       </c>
-      <c r="K26" s="28" t="s">
-        <v>105</v>
+      <c r="K26" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
@@ -1958,34 +1883,34 @@
       <c r="U26" s="2"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="20">
+      <c r="A27" s="16">
         <v>2</v>
       </c>
-      <c r="B27" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="17">
+      <c r="B27" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="14">
         <v>2</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="14">
         <v>5</v>
       </c>
-      <c r="F27" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="28">
+      <c r="F27" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="12"/>
+      <c r="I27" s="23">
         <v>2</v>
       </c>
-      <c r="J27" s="28">
+      <c r="J27" s="23">
         <v>12</v>
       </c>
-      <c r="K27" s="28" t="s">
-        <v>109</v>
+      <c r="K27" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -1996,28 +1921,28 @@
       <c r="U27" s="2"/>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="20">
+      <c r="A28" s="16">
         <v>3</v>
       </c>
-      <c r="B28" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="17">
+      <c r="B28" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="14">
         <v>3</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="14">
         <v>6</v>
       </c>
-      <c r="F28" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
+      <c r="F28" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -2031,28 +1956,28 @@
       <c r="U28" s="2"/>
     </row>
     <row r="29" spans="1:21">
-      <c r="A29" s="20">
+      <c r="A29" s="16">
         <v>4</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="17">
+      <c r="B29" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="14">
         <v>4</v>
       </c>
-      <c r="E29" s="17">
+      <c r="E29" s="14">
         <v>7</v>
       </c>
-      <c r="F29" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
+      <c r="F29" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -2066,28 +1991,28 @@
       <c r="U29" s="2"/>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="20">
+      <c r="A30" s="16">
         <v>5</v>
       </c>
-      <c r="B30" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="17">
+      <c r="B30" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="14">
         <v>5</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="14">
         <v>8</v>
       </c>
-      <c r="F30" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
+      <c r="F30" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -2101,28 +2026,28 @@
       <c r="U30" s="2"/>
     </row>
     <row r="31" spans="1:21">
-      <c r="A31" s="20">
+      <c r="A31" s="16">
         <v>6</v>
       </c>
-      <c r="B31" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="17">
+      <c r="B31" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="14">
         <v>6</v>
       </c>
-      <c r="E31" s="17">
+      <c r="E31" s="14">
         <v>9</v>
       </c>
-      <c r="F31" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
+      <c r="F31" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -2136,28 +2061,28 @@
       <c r="U31" s="2"/>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="20">
+      <c r="A32" s="16">
         <v>7</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="17">
+      <c r="B32" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="14">
         <v>7</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="14">
         <v>10</v>
       </c>
-      <c r="F32" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
+      <c r="F32" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
@@ -2171,16 +2096,16 @@
       <c r="U32" s="2"/>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33" s="20">
+      <c r="A33" s="16">
         <v>8</v>
       </c>
-      <c r="B33" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
+      <c r="B33" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -2198,21 +2123,21 @@
       <c r="U33" s="2"/>
     </row>
     <row r="34" spans="1:21">
-      <c r="A34" s="20">
+      <c r="A34" s="16">
         <v>9</v>
       </c>
-      <c r="B34" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="23"/>
+      <c r="B34" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="18"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -2227,29 +2152,29 @@
       <c r="U34" s="2"/>
     </row>
     <row r="35" spans="1:21">
-      <c r="A35" s="20">
+      <c r="A35" s="16">
         <v>10</v>
       </c>
-      <c r="B35" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F35" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="I35" s="15"/>
+      <c r="B35" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I35" s="12"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -2264,29 +2189,29 @@
       <c r="U35" s="2"/>
     </row>
     <row r="36" spans="1:21">
-      <c r="A36" s="20">
+      <c r="A36" s="16">
         <v>11</v>
       </c>
-      <c r="B36" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="13">
+      <c r="B36" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="11">
         <v>1</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="11">
         <v>7</v>
       </c>
-      <c r="F36" s="13">
+      <c r="F36" s="11">
         <v>3</v>
       </c>
-      <c r="G36" s="27">
+      <c r="G36" s="22">
         <v>43850.625</v>
       </c>
-      <c r="H36" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="I36" s="15"/>
+      <c r="H36" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I36" s="12"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -2301,29 +2226,29 @@
       <c r="U36" s="2"/>
     </row>
     <row r="37" spans="1:21">
-      <c r="A37" s="20">
+      <c r="A37" s="16">
         <v>12</v>
       </c>
-      <c r="B37" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="13">
+      <c r="B37" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="11">
         <v>2</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="11">
         <v>2</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="11">
         <v>2</v>
       </c>
-      <c r="G37" s="27">
+      <c r="G37" s="22">
         <v>43836.416666666664</v>
       </c>
-      <c r="H37" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="I37" s="15"/>
+      <c r="H37" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I37" s="12"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -2338,29 +2263,29 @@
       <c r="U37" s="2"/>
     </row>
     <row r="38" spans="1:21">
-      <c r="A38" s="20">
+      <c r="A38" s="16">
         <v>13</v>
       </c>
-      <c r="B38" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="13">
+      <c r="B38" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="11">
         <v>3</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="11">
         <v>3</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F38" s="11">
         <v>2</v>
       </c>
-      <c r="G38" s="27">
+      <c r="G38" s="22">
         <v>43868.458333333336</v>
       </c>
-      <c r="H38" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="I38" s="15"/>
+      <c r="H38" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I38" s="12"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -2375,112 +2300,112 @@
       <c r="U38" s="2"/>
     </row>
     <row r="39" spans="1:21">
-      <c r="A39" s="20">
+      <c r="A39" s="16">
         <v>14</v>
       </c>
-      <c r="B39" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="13">
+      <c r="B39" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="11">
         <v>4</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="11">
         <v>2</v>
       </c>
-      <c r="F39" s="13">
+      <c r="F39" s="11">
         <v>2</v>
       </c>
-      <c r="G39" s="27">
+      <c r="G39" s="22">
         <v>43137.416666666664</v>
       </c>
-      <c r="H39" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="I39" s="26"/>
+      <c r="H39" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="I39" s="21"/>
     </row>
     <row r="40" spans="1:21">
-      <c r="A40" s="20">
+      <c r="A40" s="16">
         <v>15</v>
       </c>
-      <c r="B40" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="13">
+      <c r="B40" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="11">
         <v>5</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E40" s="11">
         <v>4</v>
       </c>
-      <c r="F40" s="13">
+      <c r="F40" s="11">
         <v>1</v>
       </c>
-      <c r="G40" s="27">
+      <c r="G40" s="22">
         <v>43503.458333333336</v>
       </c>
-      <c r="H40" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="I40" s="26"/>
+      <c r="H40" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="I40" s="21"/>
     </row>
     <row r="41" spans="1:21">
-      <c r="A41" s="20">
+      <c r="A41" s="16">
         <v>16</v>
       </c>
-      <c r="B41" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="13">
+      <c r="B41" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="11">
         <v>6</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="11">
         <v>7</v>
       </c>
-      <c r="F41" s="13">
+      <c r="F41" s="11">
         <v>3</v>
       </c>
-      <c r="G41" s="27">
+      <c r="G41" s="22">
         <v>43898.625</v>
       </c>
-      <c r="H41" s="24" t="s">
-        <v>137</v>
+      <c r="H41" s="19" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:21">
-      <c r="A42" s="20">
+      <c r="A42" s="16">
         <v>17</v>
       </c>
-      <c r="B42" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="13">
+      <c r="B42" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="11">
         <v>7</v>
       </c>
-      <c r="E42" s="13">
+      <c r="E42" s="11">
         <v>4</v>
       </c>
-      <c r="F42" s="13">
+      <c r="F42" s="11">
         <v>1</v>
       </c>
-      <c r="G42" s="27">
+      <c r="G42" s="22">
         <v>43899.458333333336</v>
       </c>
-      <c r="H42" s="24" t="s">
-        <v>137</v>
+      <c r="H42" s="19" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:21">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
     </row>
     <row r="44" spans="1:21">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>